<commit_message>
login test cases added and log messages updated
</commit_message>
<xml_diff>
--- a/TestCases/SpotifyTestCases.xlsx
+++ b/TestCases/SpotifyTestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abgoyal\Downloads\SpotifyAPIAutomation\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4484FD1A-E316-45B0-9322-618F6B968D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBDE16D-7CF1-40C5-9D4F-E294456A57A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Test Case Title</t>
   </si>
@@ -43,13 +43,256 @@
   </si>
   <si>
     <t>Prerequisites</t>
+  </si>
+  <si>
+    <t>Test Case Number</t>
+  </si>
+  <si>
+    <t>API endpoint available</t>
+  </si>
+  <si>
+    <t>Access token is successfully generated</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Login with invalid client_id</t>
+  </si>
+  <si>
+    <t>Login with invalid client_secret</t>
+  </si>
+  <si>
+    <t>Error message: "invalid_client"</t>
+  </si>
+  <si>
+    <t>TC_001_GenerateAccessToken_01</t>
+  </si>
+  <si>
+    <t>TC_001_GenerateAccessToken_02</t>
+  </si>
+  <si>
+    <t>TC_001_GenerateAccessToken_03</t>
+  </si>
+  <si>
+    <t>TC_001_GenerateAccessToken_04</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Login with valid </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>client_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>client_secret</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Valid </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>client_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Valid </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>client_secret</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Invalid </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>client_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Valid </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>client_secret</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Valid </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>client_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Invalid </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>client_secret</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Login with invalid </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>client_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>client_secret</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Invalid </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>client_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Invalid </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>client_secret</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +304,32 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,9 +361,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,43 +651,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
-    <col min="4" max="4" width="23.21875" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
albums endpoints test data, test cases, code added
</commit_message>
<xml_diff>
--- a/TestCases/SpotifyTestCases.xlsx
+++ b/TestCases/SpotifyTestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abgoyal\Downloads\SpotifyAPIAutomation\1-automate-albums-endpoints\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A88B68F-BBF3-4530-A6FF-D0DCA62D0487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6E6BAA-E723-4C0D-98E6-AFF078B3BBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
   <si>
     <t>Test Case Title</t>
   </si>
@@ -321,9 +321,6 @@
     </r>
   </si>
   <si>
-    <t>id = "4aawyAB9vmqN3uQ7FjRGTy", market = "US"</t>
-  </si>
-  <si>
     <t>Test valid album ID with market</t>
   </si>
   <si>
@@ -386,9 +383,6 @@
   </si>
   <si>
     <t>Test with invalid market code</t>
-  </si>
-  <si>
-    <t>id = "4aawyAB9vmqN3uQ7FjRGTy", market = "XX"</t>
   </si>
   <si>
     <t>Test unauthorized request</t>
@@ -549,6 +543,23 @@
       <t>,
  error message "Only valid bearer authentication supported"</t>
     </r>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>test_GenerateAccessToken</t>
+  </si>
+  <si>
+    <t>test_getSingleAlbum</t>
+  </si>
+  <si>
+    <t>id = "4aawyAB9vmqN3uQ7FjRGTy",
+market = "US"</t>
+  </si>
+  <si>
+    <t>id = "4aawyAB9vmqN3uQ7FjRGTy",
+market = "XX"</t>
   </si>
 </sst>
 </file>
@@ -917,123 +928,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1046,180 +1073,208 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07CA67E-2E96-4DCF-B442-E130EDD2C8EC}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8">
+    <row r="2" spans="1:8" ht="28.8">
       <c r="A2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="43.2">
+      <c r="A3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="43.2">
+      <c r="A4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8">
+      <c r="A5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="28.8">
+      <c r="A6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="43.2">
+      <c r="A7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="43.2">
-      <c r="A3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="43.2">
-      <c r="A4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.8">
-      <c r="A5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.8">
-      <c r="A6" s="3" t="s">
+    <row r="8" spans="1:8" ht="28.8">
+      <c r="A8" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="43.2">
-      <c r="A7" s="3" t="s">
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8">
+      <c r="A9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="28.8">
-      <c r="A8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.8">
-      <c r="A9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get Album Tracks test cases added
</commit_message>
<xml_diff>
--- a/TestCases/SpotifyTestCases.xlsx
+++ b/TestCases/SpotifyTestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abgoyal\Downloads\SpotifyAPIAutomation\1-automate-albums-endpoints\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F793FBE-0C8A-4470-B55D-7CC11F1C2872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C42F5F-E730-4552-9659-5681EC0EE870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="113">
   <si>
     <t>Test Case Title</t>
   </si>
@@ -672,6 +672,138 @@
   </si>
   <si>
     <t>test_getMultipleAlbums</t>
+  </si>
+  <si>
+    <t>Test with valid album ID and 
+Invalid offset</t>
+  </si>
+  <si>
+    <t>Test with valid album ID and 
+Invalid limit</t>
+  </si>
+  <si>
+    <t>Test with valid album ID and 
+valid offset</t>
+  </si>
+  <si>
+    <t>id = "4aawyAB9vmqN3uQ7FjRGTy",
+offset=   ,10</t>
+  </si>
+  <si>
+    <t>id = "4aawyAB9vmqN3uQ7FjRGTy",
+limit=  ,10</t>
+  </si>
+  <si>
+    <t>Test with valid album ID and 
+valid limit</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Status Code: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>400 Bad Request</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,
+ error message "Invalid limit"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Status Code: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>400 Bad Request</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,
+ error message "Invalid offset"</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_002_Albums_22</t>
+  </si>
+  <si>
+    <t>TC_002_Albums_23</t>
+  </si>
+  <si>
+    <t>TC_002_Albums_24</t>
+  </si>
+  <si>
+    <t>TC_002_Albums_25</t>
+  </si>
+  <si>
+    <t>TC_002_Albums_26</t>
+  </si>
+  <si>
+    <t>TC_002_Albums_27</t>
+  </si>
+  <si>
+    <t>TC_002_Albums_28</t>
+  </si>
+  <si>
+    <t>TC_002_Albums_29</t>
+  </si>
+  <si>
+    <t>TC_002_Albums_30</t>
+  </si>
+  <si>
+    <t>test_getAlbumTracks</t>
+  </si>
+  <si>
+    <t>TC_002_Albums_31</t>
+  </si>
+  <si>
+    <t>TC_002_Albums_32</t>
+  </si>
+  <si>
+    <t>Test with valid album ID and 
+Below Minimum limit</t>
+  </si>
+  <si>
+    <t>id = "4aawyAB9vmqN3uQ7FjRGTy",
+limit=11.1,a</t>
+  </si>
+  <si>
+    <t>id = "4aawyAB9vmqN3uQ7FjRGTy",
+offset=11.1,a</t>
+  </si>
+  <si>
+    <t>id = "4aawyAB9vmqN3uQ7FjRGTy",
+limit=-1,0</t>
+  </si>
+  <si>
+    <t>Test with valid album ID and 
+Above Maximum limit</t>
+  </si>
+  <si>
+    <t>id = "4aawyAB9vmqN3uQ7FjRGTy",
+limit=51,100</t>
   </si>
 </sst>
 </file>
@@ -1181,11 +1313,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07CA67E-2E96-4DCF-B442-E130EDD2C8EC}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1642,6 +1774,226 @@
         <v>37</v>
       </c>
     </row>
+    <row r="23" spans="1:6" ht="28.8">
+      <c r="A23" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="43.2">
+      <c r="A24" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="43.2">
+      <c r="A25" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="28.8">
+      <c r="A26" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="28.8">
+      <c r="A27" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="28.8">
+      <c r="A28" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28.8">
+      <c r="A29" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.8">
+      <c r="A30" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28.8">
+      <c r="A31" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="28.8">
+      <c r="A32" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="28.8">
+      <c r="A33" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B33" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Artists all endpoints test cases is completed
</commit_message>
<xml_diff>
--- a/TestCases/SpotifyTestCases.xlsx
+++ b/TestCases/SpotifyTestCases.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abgoyal\Downloads\SpotifyAPIAutomation\1-automate-albums-endpoints\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abgoyal\Downloads\SpotifyAPIAutomation\3-automate-artists-endpoints\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C28895-B719-4F26-80BD-5DBEEFA9D3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C759E89B-F17F-4965-9D41-51A7BB9BC0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Albums" sheetId="2" r:id="rId2"/>
+    <sheet name="Artists" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Albums!$A$1:$G$45</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="218">
   <si>
     <t>Test Case Title</t>
   </si>
@@ -909,6 +910,345 @@
   </si>
   <si>
     <t>limit=51,100</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_01</t>
+  </si>
+  <si>
+    <t>Test with non-existent album ID</t>
+  </si>
+  <si>
+    <t>id = "0TnOYISbd1XQRBk9myaseg"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Status Code: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>400 Bad Request</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,
+error message indicating "Invalid base62 id"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Status Code: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>404 Not Found</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,
+error message indicating "Resource not found"</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_003_Artists_02</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_03</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Status Code: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>200 OK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 
+response contains album details</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Status Code: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>400 Unauthorized</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,
+error message "Only valid bearer authentication supported"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Status Code: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>401 Unauthorized</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 
+error message "Invalid access token"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Status Code: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>401 Unauthorized</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 
+error message "The access token expired"</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_003_Artists_04</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_05</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_06</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_07</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_08</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_09</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_10</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_11</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_12</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_13</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_14</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_15</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_16</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_17</t>
+  </si>
+  <si>
+    <t>test_getArtist</t>
+  </si>
+  <si>
+    <t>id = "57Pk2GU0ABFYBbbcgYxqki,6WzRpISELf3YglGAh7TXcG,6z3HAUZpAyJ0ctsbAwAiw3,6uFn47ACjqYkc0jADwEdj1,4GssB27iJeqmfGxS94Tfij,4myFsmx2v6znDOJfn3IkbD,79s5XnCN4TJKTVMSmOx8Ep,3wn8nOygkHLUQ9dlXM1rKW,6AviHKu3ydzAePBmzEi62v,6mSJEqkgiBMtqZSXSMvb4s,0widrZ6KVNuIPhbM1rWPDR,19UUPNx5jccGgQ2GCIZkww,2g8HN35AnVGIk7B8yMucww,3lOMJTQTd6J34faYwASc33,3Jv1XgMPVjdN5xGfnRJ20s,4E5IFAXCob6QqZaJMTw5YN,6EDO9iiTtwNv6waLwa1UUq,5zd9TgduWbfFXwgnm3K3Rz,4BLbZo3DCqQXMzogWV1GNP,2Ct0MnmqHDvjLqpi5gxcSM,5sbooPcNgIE22DwO0VNGUJ,3cIjeDpRUFiKU5tDXEY7Aw,5lrWzVarOIEauzOloHRCDj,0So2sgVa8aJiARPl2P29u2,43U1bCDTZAhhY1Y8mCkTG4,3xvzR05d6KgexfzjJgDRDl,53dGCRXGyCUV5Ycoy6Md34,0fIffclhgJC5h8AdMMVvkp,25zlnOAzbVoOzIeXSvQFf1,47yD0e9MCRIB8dgUXPfyW3,26Fx8UbsC0BV4J1CdtuLAy,7vGRXiYWFk6NjUnsNjQJQd,1jaTQ3nqY3oAAYyCTbIvnM,0PvFJmanyNQMseIFrU708S,1EG6y4KL5c0T5UAT41d7VH,5rZlwNFl01HqLWBQGryKSm,1tkg4EHVoqnhR6iFEXb60y,6DbqCKweKwVkHgRv1CI53D,67gUqq3wVAztSquOpNZ4Xs,25G8NNFBnjXgWCGtyPa1Ax,1jDbQz6tr52WgScCTXMnaN,5mPSyjLatqB00IkPqRlbTE,0Jc8qF1mUPo1A96HE9QxZz,5z46NBsndcpz5sdywfdqul,61N12G2IDag927XDCmMDr8,0VOMBffX1llDu37yQUt3u3,4JYFFgmy2ZZWvhCh8aZbjP,5rpkYHBqreIuzSVrYWcNa1,5KzobobnQb7UZXKOUT249o,1sbEeUY8KsdvgiQi26JBFz"</t>
+  </si>
+  <si>
+    <t>id = "2CIMQHirSU0MQqyYHq0eOx,57dN52uHvrHOxijzpIgu3E,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6,1vCWHaC5f2uS3yhpwWbIA6"</t>
+  </si>
+  <si>
+    <t>Test with more than 50 valid album 
+IDs</t>
+  </si>
+  <si>
+    <t>Test with 50 valid album IDs</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_18</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_19</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_20</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_21</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_22</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_23</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_24</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_25</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_26</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_27</t>
+  </si>
+  <si>
+    <t>test_getSeveralArtists</t>
+  </si>
+  <si>
+    <t>test_getArtistsAlbums</t>
+  </si>
+  <si>
+    <t>Test with valid market code</t>
+  </si>
+  <si>
+    <t>id = "4aawyAB9vmqN3uQ7FjRGTy",
+market = IN</t>
+  </si>
+  <si>
+    <t>Test with valid album ID and 
+Below Minimum limit (Minimum Limit is 1)</t>
+  </si>
+  <si>
+    <t>include_groups = "single"</t>
+  </si>
+  <si>
+    <t>include_groups = "single,appears_on"</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_28</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_29</t>
+  </si>
+  <si>
+    <t>Test with single include groups</t>
+  </si>
+  <si>
+    <t>Test with multiple include groups</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_30</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_31</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_32</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_33</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_34</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_35</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_36</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_37</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_38</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_39</t>
+  </si>
+  <si>
+    <t>test_getArtistsTopTracks</t>
+  </si>
+  <si>
+    <t>Test with valid market</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_40</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_41</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_42</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_43</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_44</t>
+  </si>
+  <si>
+    <t>TC_003_Artists_45</t>
+  </si>
+  <si>
+    <t>test_getArtistsRelatedArtists</t>
   </si>
 </sst>
 </file>
@@ -1420,9 +1760,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07CA67E-2E96-4DCF-B442-E130EDD2C8EC}">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2554,4 +2894,951 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4BE9265-A306-41EA-99AA-3EE3C1D4FB16}">
+  <dimension ref="A1:G46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="109.44140625" customWidth="1"/>
+    <col min="6" max="6" width="40.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="28.8">
+      <c r="A2" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.8">
+      <c r="A3" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8">
+      <c r="A4" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.2">
+      <c r="A5" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.8">
+      <c r="A6" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8">
+      <c r="A7" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.8">
+      <c r="A8" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="28.8">
+      <c r="A9" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8">
+      <c r="A10" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.8">
+      <c r="A11" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="171.6">
+      <c r="A12" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C12" t="s">
+        <v>177</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="343.2">
+      <c r="A13" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="28.8">
+      <c r="A14" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="43.2">
+      <c r="A15" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="43.2">
+      <c r="A16" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" t="s">
+        <v>188</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.8">
+      <c r="A17" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" t="s">
+        <v>188</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.8">
+      <c r="A18" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B18" t="s">
+        <v>188</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.8">
+      <c r="A19" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="28.8">
+      <c r="A20" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20" t="s">
+        <v>189</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8">
+      <c r="A21" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B21" t="s">
+        <v>189</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="28.8">
+      <c r="A22" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B22" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.8">
+      <c r="A23" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B23" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="28.8">
+      <c r="A24" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B24" t="s">
+        <v>189</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="28.8">
+      <c r="A25" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B25" t="s">
+        <v>189</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="28.8">
+      <c r="A26" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="43.2">
+      <c r="A27" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27" t="s">
+        <v>189</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="43.2">
+      <c r="A28" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B28" t="s">
+        <v>189</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28.8">
+      <c r="A29" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B29" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.8">
+      <c r="A30" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" t="s">
+        <v>189</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="43.2">
+      <c r="A31" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B31" t="s">
+        <v>189</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="28.8">
+      <c r="A32" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="28.8">
+      <c r="A33" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B33" t="s">
+        <v>189</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.8">
+      <c r="A34" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B34" t="s">
+        <v>209</v>
+      </c>
+      <c r="C34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="28.8">
+      <c r="A35" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B35" t="s">
+        <v>209</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="28.8">
+      <c r="A36" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B36" t="s">
+        <v>209</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="28.8">
+      <c r="A37" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B37" t="s">
+        <v>209</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="43.2">
+      <c r="A38" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B38" t="s">
+        <v>209</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E38" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="28.8">
+      <c r="A39" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B39" t="s">
+        <v>209</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="28.8">
+      <c r="A40" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B40" t="s">
+        <v>209</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="28.8">
+      <c r="A41" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B41" t="s">
+        <v>217</v>
+      </c>
+      <c r="C41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" t="s">
+        <v>23</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="28.8">
+      <c r="A42" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B42" t="s">
+        <v>217</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="28.8">
+      <c r="A43" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B43" t="s">
+        <v>217</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="43.2">
+      <c r="A44" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B44" t="s">
+        <v>217</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="28.8">
+      <c r="A45" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B45" t="s">
+        <v>217</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E45" t="s">
+        <v>23</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="28.8">
+      <c r="A46" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B46" t="s">
+        <v>217</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" t="s">
+        <v>23</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>